<commit_message>
add a couple more packages
</commit_message>
<xml_diff>
--- a/doc/CTV ClinicalTrial File.xlsx
+++ b/doc/CTV ClinicalTrial File.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ywang10\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ywang10\GitHubPkgs\CRAN-task-view-ClinicalTrials\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11CF9FB0-3286-40DB-B5E6-FDB474ABD2F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{415F56E8-2226-4362-A4DB-C1591FAE9818}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-12" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="259">
   <si>
     <t>Package Name</t>
   </si>
@@ -204,9 +204,6 @@
     <t>Monitoring</t>
   </si>
   <si>
-    <t>`r pkg("monitOS") Monitoring Overall Survival in Pivotal Trials in Indolent Cancers</t>
-  </si>
-  <si>
     <t>OncoBayes2</t>
   </si>
   <si>
@@ -513,9 +510,6 @@
     <t>adpss</t>
   </si>
   <si>
-    <t>Provides the functions for planning and conducting a clinical trial with adaptive sample size determination. Maximal statistical efficiency will be exploited even when dramatic or multiple adaptations are made. Such a trial consists of adaptive determination of sample size at an interim analysis and implementation of frequentist statistical test at the interim and final analysis with a prefixed significance level. The required assumptions for the stage-wise test statistics are independent and stationary increments and normality. Predetermination of adaptation rule is not required.</t>
-  </si>
-  <si>
     <t>ASSISTant</t>
   </si>
   <si>
@@ -678,9 +672,6 @@
     <t>`r pkg("iAdapt")` Simulate and implement early phase two-stage adaptive dose-finding design for binary and quasi-continuous toxicity endpoints. See Chiuzan et al. (2018) for further reading &lt;doi:10.1080/19466315.2018.1462727&gt;.</t>
   </si>
   <si>
-    <t>`r pkg("OncoBayes")` Bayesian Logistic Regression for Oncology Dose-Escalation Trials.</t>
-  </si>
-  <si>
     <t>`r pkg("clinfun", priority = "core")` has functions for both design and analysis of clinical trials. For phase II trials, it has functions to calculate sample size, effect size, and power based on Fisher's exact test, the operating characteristics of a two-stage boundary, Optimal and Minimax 2-stage Phase II designs given by Richard Simon, the exact 1-stage Phase II design and can compute a stopping rule and its operating characteristics for toxicity monitoring based repeated significance testing. For phase III trials, it can calculate sample size for group sequential designs.</t>
   </si>
   <si>
@@ -805,6 +796,15 @@
   </si>
   <si>
     <t>Adaptive designs, Monitoring, Simulation</t>
+  </si>
+  <si>
+    <t>`r pkg("adpss")` provides the functions for planning and conducting a clinical trial with adaptive sample size determination. Maximal statistical efficiency will be exploited even when dramatic or multiple adaptations are made. Such a trial consists of adaptive determination of sample size at an interim analysis and implementation of frequentist statistical test at the interim and final analysis with a prefixed significance level. The required assumptions for the stage-wise test statistics are independent and stationary increments and normality. Predetermination of adaptation rule is not required.</t>
+  </si>
+  <si>
+    <t>`r pkg("monitOS") Monitoring Overall Survival in Pivotal Trials in Indolent Cancers.</t>
+  </si>
+  <si>
+    <t>`r pkg("OncoBayes2")` Bayesian Logistic Regression for Oncology Dose-Escalation Trials.</t>
   </si>
 </sst>
 </file>
@@ -1197,21 +1197,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1006"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="F71" sqref="F71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.109375" customWidth="1"/>
-    <col min="5" max="5" width="26.5546875" style="16" customWidth="1"/>
-    <col min="6" max="6" width="168" style="16" customWidth="1"/>
-    <col min="7" max="7" width="116.6640625" style="16" customWidth="1"/>
-    <col min="8" max="8" width="17.5546875" customWidth="1"/>
-    <col min="9" max="26" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.08984375" customWidth="1"/>
+    <col min="5" max="5" width="26.54296875" style="16" customWidth="1"/>
+    <col min="6" max="6" width="171.90625" style="16" customWidth="1"/>
+    <col min="7" max="7" width="116.6328125" style="16" customWidth="1"/>
+    <col min="8" max="8" width="17.54296875" customWidth="1"/>
+    <col min="9" max="26" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26">
@@ -1228,7 +1228,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>4</v>
@@ -1258,144 +1258,144 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="43.2">
+    <row r="2" spans="1:26" ht="43.5">
       <c r="A2" s="26" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>26</v>
       </c>
       <c r="C2" s="12"/>
       <c r="D2" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F2" s="23" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="G2" s="7"/>
     </row>
     <row r="3" spans="1:26">
       <c r="A3" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="F3" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="F3" s="20" t="s">
-        <v>102</v>
-      </c>
       <c r="G3" s="7"/>
     </row>
-    <row r="4" spans="1:26" ht="43.2">
+    <row r="4" spans="1:26" ht="43.5">
       <c r="A4" s="25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="F4" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="E4" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>100</v>
-      </c>
       <c r="G4" s="7"/>
     </row>
-    <row r="5" spans="1:26" ht="28.8">
+    <row r="5" spans="1:26" ht="29">
       <c r="A5" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>26</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G5" s="7"/>
     </row>
     <row r="6" spans="1:26">
       <c r="A6" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>26</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G6" s="7"/>
     </row>
     <row r="7" spans="1:26">
       <c r="A7" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>26</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G7" s="7"/>
     </row>
     <row r="8" spans="1:26">
       <c r="A8" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G8" s="7"/>
     </row>
     <row r="9" spans="1:26">
       <c r="A9" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>26</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E9" s="7"/>
       <c r="F9" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G9" s="7"/>
     </row>
     <row r="10" spans="1:26">
       <c r="A10" s="8" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>26</v>
@@ -1405,16 +1405,16 @@
         <v>47</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="G10" s="7"/>
     </row>
     <row r="11" spans="1:26">
       <c r="A11" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>26</v>
@@ -1423,16 +1423,16 @@
         <v>47</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="G11" s="7"/>
     </row>
     <row r="12" spans="1:26">
       <c r="A12" s="8" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>26</v>
@@ -1442,16 +1442,16 @@
         <v>47</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="G12" s="7"/>
     </row>
     <row r="13" spans="1:26">
       <c r="A13" s="8" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>26</v>
@@ -1461,16 +1461,16 @@
         <v>47</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:26">
       <c r="A14" s="8" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>26</v>
@@ -1480,16 +1480,16 @@
         <v>47</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="G14" s="7"/>
     </row>
-    <row r="15" spans="1:26" ht="28.8">
+    <row r="15" spans="1:26" ht="29">
       <c r="A15" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>26</v>
@@ -1498,16 +1498,16 @@
         <v>47</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="G15" s="7"/>
     </row>
-    <row r="16" spans="1:26" ht="28.8">
+    <row r="16" spans="1:26" ht="29">
       <c r="A16" s="8" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>26</v>
@@ -1517,16 +1517,16 @@
         <v>47</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="G16" s="7"/>
     </row>
-    <row r="17" spans="1:26" ht="28.8">
+    <row r="17" spans="1:26" ht="29">
       <c r="A17" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>26</v>
@@ -1538,13 +1538,13 @@
         <v>57</v>
       </c>
       <c r="F17" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="G17" s="7"/>
+    </row>
+    <row r="18" spans="1:26" ht="29">
+      <c r="A18" s="5" t="s">
         <v>115</v>
-      </c>
-      <c r="G17" s="7"/>
-    </row>
-    <row r="18" spans="1:26" ht="28.8">
-      <c r="A18" s="5" t="s">
-        <v>116</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>22</v>
@@ -1556,13 +1556,13 @@
         <v>11</v>
       </c>
       <c r="F18" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="G18" s="7"/>
+    </row>
+    <row r="19" spans="1:26" ht="29">
+      <c r="A19" s="5" t="s">
         <v>117</v>
-      </c>
-      <c r="G18" s="7"/>
-    </row>
-    <row r="19" spans="1:26" ht="28.8">
-      <c r="A19" s="5" t="s">
-        <v>118</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>26</v>
@@ -1572,13 +1572,13 @@
       </c>
       <c r="E19" s="7"/>
       <c r="F19" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G19" s="7"/>
     </row>
-    <row r="20" spans="1:26" ht="28.8">
+    <row r="20" spans="1:26" ht="29">
       <c r="A20" s="8" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>26</v>
@@ -1588,10 +1588,10 @@
         <v>47</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="G20" s="21"/>
       <c r="H20" s="22"/>
@@ -1616,7 +1616,7 @@
     </row>
     <row r="21" spans="1:26">
       <c r="A21" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>26</v>
@@ -1626,16 +1626,16 @@
         <v>47</v>
       </c>
       <c r="E21" s="17" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F21" s="19" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="G21" s="7"/>
     </row>
-    <row r="22" spans="1:26" ht="28.8">
+    <row r="22" spans="1:26" ht="29">
       <c r="A22" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>8</v>
@@ -1644,16 +1644,16 @@
         <v>47</v>
       </c>
       <c r="E22" s="17" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G22" s="7"/>
     </row>
     <row r="23" spans="1:26">
       <c r="A23" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>26</v>
@@ -1663,13 +1663,13 @@
       </c>
       <c r="E23" s="7"/>
       <c r="F23" s="7" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G23" s="7"/>
     </row>
     <row r="24" spans="1:26">
       <c r="A24" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>26</v>
@@ -1679,13 +1679,13 @@
       </c>
       <c r="E24" s="6"/>
       <c r="F24" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G24" s="7"/>
     </row>
     <row r="25" spans="1:26">
       <c r="A25" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>26</v>
@@ -1695,11 +1695,11 @@
       </c>
       <c r="E25" s="7"/>
       <c r="F25" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G25" s="7"/>
     </row>
-    <row r="26" spans="1:26" ht="43.2">
+    <row r="26" spans="1:26" ht="43.5">
       <c r="A26" s="5" t="s">
         <v>44</v>
       </c>
@@ -1711,16 +1711,16 @@
         <v>47</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="G26" s="7"/>
     </row>
     <row r="27" spans="1:26">
       <c r="A27" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B27" s="8" t="s">
         <v>26</v>
@@ -1731,13 +1731,13 @@
       </c>
       <c r="E27" s="8"/>
       <c r="F27" s="9" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="G27" s="7"/>
     </row>
-    <row r="28" spans="1:26" ht="28.8">
+    <row r="28" spans="1:26" ht="29">
       <c r="A28" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B28" s="8" t="s">
         <v>26</v>
@@ -1748,13 +1748,13 @@
       </c>
       <c r="E28" s="8"/>
       <c r="F28" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G28" s="7"/>
     </row>
-    <row r="29" spans="1:26" ht="28.8">
+    <row r="29" spans="1:26" ht="29">
       <c r="A29" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>26</v>
@@ -1763,16 +1763,16 @@
         <v>47</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G29" s="7"/>
     </row>
     <row r="30" spans="1:26">
       <c r="A30" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B30" s="8" t="s">
         <v>26</v>
@@ -1782,16 +1782,16 @@
         <v>47</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="G30" s="7"/>
     </row>
-    <row r="31" spans="1:26" ht="28.8">
+    <row r="31" spans="1:26" ht="29">
       <c r="A31" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>26</v>
@@ -1803,13 +1803,13 @@
         <v>11</v>
       </c>
       <c r="F31" s="20" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G31" s="7"/>
     </row>
-    <row r="32" spans="1:26" ht="28.8">
+    <row r="32" spans="1:26" ht="29">
       <c r="A32" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>26</v>
@@ -1819,13 +1819,13 @@
       </c>
       <c r="E32" s="7"/>
       <c r="F32" s="7" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G32" s="7"/>
     </row>
-    <row r="33" spans="1:26" ht="43.2">
+    <row r="33" spans="1:26" ht="43.5">
       <c r="A33" s="12" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="B33" s="12" t="s">
         <v>26</v>
@@ -1836,13 +1836,13 @@
       </c>
       <c r="E33" s="14"/>
       <c r="F33" s="13" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G33" s="7"/>
     </row>
     <row r="34" spans="1:26">
       <c r="A34" s="8" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B34" s="8" t="s">
         <v>26</v>
@@ -1852,10 +1852,10 @@
         <v>10</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="F34" s="9" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G34" s="15"/>
       <c r="H34" s="10"/>
@@ -1878,679 +1878,679 @@
       <c r="Y34" s="10"/>
       <c r="Z34" s="10"/>
     </row>
-    <row r="35" spans="1:26" ht="172.8">
+    <row r="35" spans="1:26" ht="174">
       <c r="A35" s="12" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B35" s="12" t="s">
         <v>26</v>
       </c>
       <c r="C35" s="12"/>
       <c r="D35" s="12" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E35" s="23" t="s">
         <v>51</v>
       </c>
       <c r="F35" s="14" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="G35" s="7"/>
     </row>
-    <row r="36" spans="1:26" ht="28.8">
+    <row r="36" spans="1:26" ht="29">
       <c r="A36" s="26" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B36" s="12" t="s">
         <v>26</v>
       </c>
       <c r="C36" s="12"/>
       <c r="D36" s="12" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E36" s="14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F36" s="23" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="G36" s="7"/>
     </row>
-    <row r="37" spans="1:26" ht="28.8">
+    <row r="37" spans="1:26" ht="29">
       <c r="A37" s="12" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B37" s="12" t="s">
         <v>26</v>
       </c>
       <c r="C37" s="12"/>
       <c r="D37" s="12" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E37" s="14" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="F37" s="14" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="G37" s="7"/>
     </row>
-    <row r="38" spans="1:26" ht="57.6">
+    <row r="38" spans="1:26" ht="58">
       <c r="A38" s="26" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B38" s="12" t="s">
         <v>26</v>
       </c>
       <c r="C38" s="12"/>
       <c r="D38" s="12" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E38" s="14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F38" s="23" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G38" s="7"/>
     </row>
-    <row r="39" spans="1:26" ht="28.8">
+    <row r="39" spans="1:26" ht="29">
       <c r="A39" s="12" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B39" s="12" t="s">
         <v>26</v>
       </c>
       <c r="C39" s="12"/>
       <c r="D39" s="12" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E39" s="14" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F39" s="14" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="G39" s="7"/>
     </row>
-    <row r="40" spans="1:26" ht="72">
+    <row r="40" spans="1:26" ht="72.5">
       <c r="A40" s="12" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B40" s="12" t="s">
         <v>26</v>
       </c>
       <c r="C40" s="12"/>
       <c r="D40" s="12" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E40" s="14" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F40" s="14" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="G40" s="7"/>
     </row>
-    <row r="41" spans="1:26" ht="57.6">
+    <row r="41" spans="1:26" ht="58">
       <c r="A41" s="12" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B41" s="12" t="s">
         <v>26</v>
       </c>
       <c r="C41" s="12"/>
       <c r="D41" s="12" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E41" s="14" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F41" s="14" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="G41" s="7"/>
     </row>
-    <row r="42" spans="1:26" ht="28.8">
+    <row r="42" spans="1:26" ht="29">
       <c r="A42" s="12" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B42" s="12" t="s">
         <v>26</v>
       </c>
       <c r="C42" s="12"/>
       <c r="D42" s="12" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E42" s="14" t="s">
         <v>16</v>
       </c>
       <c r="F42" s="14" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G42" s="7"/>
     </row>
-    <row r="43" spans="1:26" ht="115.2">
+    <row r="43" spans="1:26" ht="116">
       <c r="A43" s="12" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B43" s="12" t="s">
         <v>26</v>
       </c>
       <c r="C43" s="12"/>
       <c r="D43" s="12" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E43" s="14" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F43" s="14" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="G43" s="7"/>
     </row>
-    <row r="44" spans="1:26" ht="28.8">
+    <row r="44" spans="1:26" ht="29">
       <c r="A44" s="12" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B44" s="12" t="s">
         <v>26</v>
       </c>
       <c r="C44" s="12"/>
       <c r="D44" s="12" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E44" s="14" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F44" s="14" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="G44" s="7"/>
     </row>
-    <row r="45" spans="1:26" ht="28.8">
+    <row r="45" spans="1:26" ht="29">
       <c r="A45" s="12" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B45" s="12" t="s">
         <v>26</v>
       </c>
       <c r="C45" s="12"/>
       <c r="D45" s="12" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E45" s="14" t="s">
         <v>16</v>
       </c>
       <c r="F45" s="14" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="G45" s="7"/>
     </row>
-    <row r="46" spans="1:26" ht="86.4">
+    <row r="46" spans="1:26" ht="87">
       <c r="A46" s="12" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B46" s="12" t="s">
         <v>26</v>
       </c>
       <c r="C46" s="12"/>
       <c r="D46" s="12" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E46" s="14" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F46" s="14" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="G46" s="7"/>
     </row>
-    <row r="47" spans="1:26" ht="72">
+    <row r="47" spans="1:26" ht="72.5">
       <c r="A47" s="12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B47" s="12" t="s">
         <v>26</v>
       </c>
       <c r="C47" s="12"/>
       <c r="D47" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E47" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F47" s="14" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="G47" s="7"/>
     </row>
-    <row r="48" spans="1:26" ht="43.2">
+    <row r="48" spans="1:26" ht="43.5">
       <c r="A48" s="12" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B48" s="12" t="s">
         <v>26</v>
       </c>
       <c r="C48" s="12"/>
       <c r="D48" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E48" s="14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F48" s="14" t="s">
-        <v>161</v>
+        <v>256</v>
       </c>
       <c r="G48" s="7"/>
     </row>
-    <row r="49" spans="1:7" ht="28.8">
+    <row r="49" spans="1:7" ht="29">
       <c r="A49" s="26" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B49" s="12" t="s">
         <v>26</v>
       </c>
       <c r="C49" s="12"/>
       <c r="D49" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E49" s="14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F49" s="23" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="G49" s="7"/>
     </row>
-    <row r="50" spans="1:7" ht="57.6">
+    <row r="50" spans="1:7" ht="58">
       <c r="A50" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B50" s="8" t="s">
         <v>26</v>
       </c>
       <c r="C50" s="8"/>
       <c r="D50" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E50" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F50" s="9" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="G50" s="7"/>
     </row>
     <row r="51" spans="1:7">
       <c r="A51" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B51" s="8" t="s">
         <v>26</v>
       </c>
       <c r="C51" s="8"/>
       <c r="D51" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F51" s="9" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="G51" s="7"/>
     </row>
     <row r="52" spans="1:7">
       <c r="A52" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B52" s="8" t="s">
         <v>26</v>
       </c>
       <c r="C52" s="8"/>
       <c r="D52" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E52" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F52" s="9" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="G52" s="7"/>
     </row>
-    <row r="53" spans="1:7" ht="43.2">
+    <row r="53" spans="1:7" ht="43.5">
       <c r="A53" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B53" s="8" t="s">
         <v>26</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E53" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F53" s="9" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G53" s="9"/>
     </row>
-    <row r="54" spans="1:7" ht="28.8">
+    <row r="54" spans="1:7" ht="29">
       <c r="A54" s="25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B54" s="5" t="s">
         <v>22</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="F54" s="20" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="G54" s="7"/>
     </row>
-    <row r="55" spans="1:7" ht="43.2">
+    <row r="55" spans="1:7" ht="43.5">
       <c r="A55" s="26" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B55" s="12" t="s">
         <v>26</v>
       </c>
       <c r="C55" s="12"/>
       <c r="D55" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E55" s="14" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F55" s="23" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G55" s="7"/>
     </row>
-    <row r="56" spans="1:7" ht="86.4">
+    <row r="56" spans="1:7" ht="87">
       <c r="A56" s="26" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B56" s="12" t="s">
         <v>26</v>
       </c>
       <c r="C56" s="12"/>
       <c r="D56" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E56" s="14" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F56" s="23" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G56" s="7"/>
     </row>
     <row r="57" spans="1:7">
       <c r="A57" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B57" s="5" t="s">
         <v>26</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E57" s="7" t="s">
         <v>16</v>
       </c>
       <c r="F57" s="7" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G57" s="7"/>
     </row>
-    <row r="58" spans="1:7" ht="43.2">
+    <row r="58" spans="1:7" ht="43.5">
       <c r="A58" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B58" s="5" t="s">
         <v>26</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E58" s="7" t="s">
         <v>16</v>
       </c>
       <c r="F58" s="7" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="G58" s="7"/>
     </row>
-    <row r="59" spans="1:7" ht="43.2">
+    <row r="59" spans="1:7" ht="43.5">
       <c r="A59" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B59" s="5" t="s">
         <v>26</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E59" s="7" t="s">
         <v>16</v>
       </c>
       <c r="F59" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G59" s="7"/>
     </row>
-    <row r="60" spans="1:7" ht="86.4">
+    <row r="60" spans="1:7" ht="87">
       <c r="A60" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B60" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E60" s="7" t="s">
         <v>16</v>
       </c>
       <c r="F60" s="7" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="G60" s="7"/>
     </row>
-    <row r="61" spans="1:7" ht="86.4">
+    <row r="61" spans="1:7" ht="87">
       <c r="A61" s="12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B61" s="12" t="s">
         <v>26</v>
       </c>
       <c r="C61" s="12"/>
       <c r="D61" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E61" s="14" t="s">
         <v>16</v>
       </c>
       <c r="F61" s="14" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G61" s="7"/>
     </row>
     <row r="62" spans="1:7">
       <c r="A62" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B62" s="12" t="s">
         <v>26</v>
       </c>
       <c r="C62" s="12"/>
       <c r="D62" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E62" s="14" t="s">
         <v>16</v>
       </c>
       <c r="F62" s="14" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="G62" s="7"/>
     </row>
-    <row r="63" spans="1:7" ht="100.8">
+    <row r="63" spans="1:7" ht="101.5">
       <c r="A63" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B63" s="5" t="s">
         <v>26</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E63" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F63" s="7" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="G63" s="7"/>
     </row>
-    <row r="64" spans="1:7" ht="43.2">
+    <row r="64" spans="1:7" ht="43.5">
       <c r="A64" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B64" s="5" t="s">
         <v>22</v>
       </c>
       <c r="D64" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E64" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="F64" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="G64" s="7"/>
+    </row>
+    <row r="65" spans="1:26" ht="43.5">
+      <c r="A65" s="5" t="s">
         <v>85</v>
-      </c>
-      <c r="E64" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="F64" s="7" t="s">
-        <v>208</v>
-      </c>
-      <c r="G64" s="7"/>
-    </row>
-    <row r="65" spans="1:26" ht="43.2">
-      <c r="A65" s="5" t="s">
-        <v>86</v>
       </c>
       <c r="B65" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E65" s="7" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F65" s="7" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="G65" s="7"/>
     </row>
-    <row r="66" spans="1:26" ht="35.4">
+    <row r="66" spans="1:26" ht="35.5">
       <c r="A66" s="18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B66" s="8" t="s">
         <v>26</v>
       </c>
       <c r="C66" s="8"/>
       <c r="D66" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E66" s="24" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F66" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G66" s="11" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="67" spans="1:26" ht="28.8">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="67" spans="1:26" ht="29">
       <c r="A67" s="12" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B67" s="12" t="s">
         <v>26</v>
       </c>
       <c r="C67" s="12"/>
       <c r="D67" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E67" s="14" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F67" s="14" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G67" s="7"/>
     </row>
-    <row r="68" spans="1:26" ht="57.6">
+    <row r="68" spans="1:26" ht="58">
       <c r="A68" s="12" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B68" s="12" t="s">
         <v>26</v>
       </c>
       <c r="C68" s="12"/>
       <c r="D68" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E68" s="14" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F68" s="14" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="G68" s="7"/>
     </row>
-    <row r="69" spans="1:26" ht="28.8">
+    <row r="69" spans="1:26" ht="29">
       <c r="A69" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B69" s="5" t="s">
         <v>26</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E69" s="20" t="s">
         <v>51</v>
       </c>
       <c r="F69" s="7" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="G69" s="7"/>
     </row>
-    <row r="70" spans="1:26" ht="28.8">
+    <row r="70" spans="1:26" ht="29">
       <c r="A70" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B70" s="12" t="s">
         <v>26</v>
       </c>
       <c r="C70" s="12"/>
       <c r="D70" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E70" s="14" t="s">
         <v>54</v>
       </c>
       <c r="F70" s="14" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="G70" s="7"/>
     </row>
@@ -2610,7 +2610,7 @@
       <c r="Y72"/>
       <c r="Z72"/>
     </row>
-    <row r="73" spans="1:26" ht="57.6">
+    <row r="73" spans="1:26" ht="58">
       <c r="A73" s="5" t="s">
         <v>29</v>
       </c>
@@ -2646,7 +2646,7 @@
       </c>
       <c r="G74" s="7"/>
     </row>
-    <row r="75" spans="1:26" ht="43.2">
+    <row r="75" spans="1:26" ht="43.5">
       <c r="A75" s="5" t="s">
         <v>36</v>
       </c>
@@ -2664,7 +2664,7 @@
       </c>
       <c r="G75" s="7"/>
     </row>
-    <row r="76" spans="1:26" ht="28.8">
+    <row r="76" spans="1:26" ht="29">
       <c r="A76" s="25" t="s">
         <v>13</v>
       </c>
@@ -2675,13 +2675,13 @@
         <v>9</v>
       </c>
       <c r="E76" s="7" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="F76" s="7" t="s">
         <v>14</v>
       </c>
       <c r="G76" s="20" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="77" spans="1:26">
@@ -2702,7 +2702,7 @@
       </c>
       <c r="G77" s="7"/>
     </row>
-    <row r="78" spans="1:26" ht="43.2">
+    <row r="78" spans="1:26" ht="43.5">
       <c r="A78" s="5" t="s">
         <v>42</v>
       </c>
@@ -2720,7 +2720,7 @@
       </c>
       <c r="G78" s="7"/>
     </row>
-    <row r="79" spans="1:26" ht="28.8">
+    <row r="79" spans="1:26" ht="29">
       <c r="A79" s="5" t="s">
         <v>44</v>
       </c>
@@ -2734,16 +2734,16 @@
         <v>9</v>
       </c>
       <c r="E79" s="20" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F79" s="7" t="s">
         <v>46</v>
       </c>
       <c r="G79" s="7" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="80" spans="1:26" ht="28.8">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="80" spans="1:26" ht="43.5">
       <c r="A80" s="5" t="s">
         <v>21</v>
       </c>
@@ -2772,14 +2772,14 @@
         <v>9</v>
       </c>
       <c r="E81" s="20" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F81" s="7" t="s">
         <v>49</v>
       </c>
       <c r="G81" s="7"/>
     </row>
-    <row r="82" spans="1:7" ht="28.8">
+    <row r="82" spans="1:7" ht="29">
       <c r="A82" s="5" t="s">
         <v>31</v>
       </c>
@@ -2807,15 +2807,17 @@
       <c r="D83" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E83" s="8"/>
+      <c r="E83" s="8" t="s">
+        <v>57</v>
+      </c>
       <c r="F83" s="9" t="s">
-        <v>58</v>
+        <v>257</v>
       </c>
       <c r="G83" s="7"/>
     </row>
     <row r="84" spans="1:7">
       <c r="A84" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B84" s="8" t="s">
         <v>26</v>
@@ -2823,15 +2825,15 @@
       <c r="D84" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E84" s="10" t="s">
+      <c r="E84" s="8" t="s">
         <v>16</v>
       </c>
       <c r="F84" s="9" t="s">
-        <v>216</v>
+        <v>258</v>
       </c>
       <c r="G84" s="7"/>
     </row>
-    <row r="85" spans="1:7" ht="28.8">
+    <row r="85" spans="1:7" ht="29">
       <c r="A85" s="5" t="s">
         <v>15</v>
       </c>
@@ -2842,14 +2844,14 @@
         <v>9</v>
       </c>
       <c r="E85" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F85" s="7" t="s">
         <v>17</v>
       </c>
       <c r="G85" s="7"/>
     </row>
-    <row r="86" spans="1:7" ht="28.8">
+    <row r="86" spans="1:7" ht="29">
       <c r="A86" s="5" t="s">
         <v>50</v>
       </c>
@@ -2867,9 +2869,9 @@
       </c>
       <c r="G86" s="7"/>
     </row>
-    <row r="87" spans="1:7" ht="43.2">
+    <row r="87" spans="1:7" ht="43.5">
       <c r="A87" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B87" s="5" t="s">
         <v>26</v>
@@ -2881,13 +2883,13 @@
         <v>51</v>
       </c>
       <c r="F87" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G87" s="7"/>
     </row>
-    <row r="88" spans="1:7" ht="28.8">
+    <row r="88" spans="1:7" ht="29">
       <c r="A88" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B88" s="5" t="s">
         <v>26</v>
@@ -2899,13 +2901,13 @@
         <v>19</v>
       </c>
       <c r="F88" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G88" s="7"/>
     </row>
-    <row r="89" spans="1:7" ht="43.2">
+    <row r="89" spans="1:7" ht="43.5">
       <c r="A89" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B89" s="5" t="s">
         <v>8</v>
@@ -2914,16 +2916,16 @@
         <v>9</v>
       </c>
       <c r="E89" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F89" s="7" t="s">
         <v>61</v>
-      </c>
-      <c r="F89" s="7" t="s">
-        <v>62</v>
       </c>
       <c r="G89" s="7"/>
     </row>
     <row r="90" spans="1:7">
       <c r="A90" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B90" s="5" t="s">
         <v>8</v>
@@ -2935,13 +2937,13 @@
         <v>23</v>
       </c>
       <c r="F90" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G90" s="7"/>
     </row>
-    <row r="91" spans="1:7" ht="28.8">
+    <row r="91" spans="1:7" ht="29">
       <c r="A91" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B91" s="5" t="s">
         <v>26</v>
@@ -2953,13 +2955,13 @@
         <v>11</v>
       </c>
       <c r="F91" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G91" s="7"/>
     </row>
     <row r="92" spans="1:7">
       <c r="A92" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B92" s="5" t="s">
         <v>26</v>
@@ -2971,11 +2973,11 @@
         <v>11</v>
       </c>
       <c r="F92" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G92" s="7"/>
     </row>
-    <row r="93" spans="1:7" ht="43.2">
+    <row r="93" spans="1:7" ht="43.5">
       <c r="A93" s="5" t="s">
         <v>38</v>
       </c>
@@ -2986,16 +2988,16 @@
         <v>9</v>
       </c>
       <c r="E93" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F93" s="7" t="s">
         <v>39</v>
       </c>
       <c r="G93" s="7"/>
     </row>
-    <row r="94" spans="1:7" ht="43.2">
+    <row r="94" spans="1:7" ht="43.5">
       <c r="A94" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B94" s="5" t="s">
         <v>26</v>
@@ -3004,14 +3006,14 @@
         <v>9</v>
       </c>
       <c r="E94" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F94" s="7" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="G94" s="7"/>
     </row>
-    <row r="95" spans="1:7" ht="43.2">
+    <row r="95" spans="1:7" ht="43.5">
       <c r="A95" s="5" t="s">
         <v>53</v>
       </c>
@@ -3029,9 +3031,9 @@
       </c>
       <c r="G95" s="7"/>
     </row>
-    <row r="96" spans="1:7" ht="43.2">
+    <row r="96" spans="1:7" ht="43.5">
       <c r="A96" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B96" s="5" t="s">
         <v>26</v>
@@ -3040,14 +3042,14 @@
         <v>9</v>
       </c>
       <c r="E96" s="20" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F96" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G96" s="7"/>
     </row>
-    <row r="97" spans="1:7">
+    <row r="97" spans="1:7" ht="29">
       <c r="A97" s="5" t="s">
         <v>7</v>
       </c>
@@ -3065,9 +3067,9 @@
       </c>
       <c r="G97" s="7"/>
     </row>
-    <row r="98" spans="1:7" ht="43.2">
+    <row r="98" spans="1:7" ht="58">
       <c r="A98" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B98" s="5" t="s">
         <v>26</v>
@@ -3079,16 +3081,16 @@
         <v>9</v>
       </c>
       <c r="E98" s="7" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="F98" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G98" s="7"/>
     </row>
-    <row r="99" spans="1:7" ht="28.8">
+    <row r="99" spans="1:7" ht="29">
       <c r="A99" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B99" s="5" t="s">
         <v>26</v>
@@ -3100,13 +3102,13 @@
         <v>54</v>
       </c>
       <c r="F99" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="G99" s="7"/>
+    </row>
+    <row r="100" spans="1:7" ht="43.5">
+      <c r="A100" s="5" t="s">
         <v>81</v>
-      </c>
-      <c r="G99" s="7"/>
-    </row>
-    <row r="100" spans="1:7" ht="43.2">
-      <c r="A100" s="5" t="s">
-        <v>82</v>
       </c>
       <c r="B100" s="5" t="s">
         <v>26</v>
@@ -3115,90 +3117,90 @@
         <v>9</v>
       </c>
       <c r="E100" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F100" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G100" s="7"/>
     </row>
     <row r="101" spans="1:7">
       <c r="A101" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B101" s="5" t="s">
         <v>26</v>
       </c>
       <c r="D101" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E101" s="20"/>
       <c r="F101" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="G101" s="7"/>
+    </row>
+    <row r="102" spans="1:7" ht="29">
+      <c r="A102" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="G101" s="7"/>
-    </row>
-    <row r="102" spans="1:7" ht="28.8">
-      <c r="A102" s="5" t="s">
-        <v>147</v>
-      </c>
       <c r="B102" s="5" t="s">
         <v>26</v>
       </c>
       <c r="D102" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E102" s="7"/>
       <c r="F102" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G102" s="7"/>
     </row>
     <row r="103" spans="1:7">
       <c r="A103" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B103" s="5" t="s">
         <v>26</v>
       </c>
       <c r="D103" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E103" s="7"/>
       <c r="F103" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G103" s="7"/>
     </row>
     <row r="104" spans="1:7">
       <c r="A104" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B104" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D104" s="5" t="s">
         <v>142</v>
-      </c>
-      <c r="B104" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D104" s="5" t="s">
-        <v>143</v>
       </c>
       <c r="E104" s="7"/>
       <c r="F104" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G104" s="7"/>
     </row>
-    <row r="105" spans="1:7" ht="28.8">
+    <row r="105" spans="1:7" ht="29">
       <c r="A105" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B105" s="5" t="s">
         <v>26</v>
       </c>
       <c r="D105" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E105" s="7"/>
       <c r="F105" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G105" s="7"/>
     </row>

</xml_diff>

<commit_message>
Update MD description and minor change to Excel Table
</commit_message>
<xml_diff>
--- a/doc/CTV ClinicalTrial File.xlsx
+++ b/doc/CTV ClinicalTrial File.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elias/Projects/CRAN-task-view-ClinicalTrials/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6F5A437-92CC-ED4D-A413-1DA9381C73FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D8B7340-D134-6246-AA37-52C15A9846E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1020" yWindow="500" windowWidth="37380" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -831,10 +831,10 @@
     <t>`r pkg("NCC")`is an R package that allows users to simulate platform trials and perform treatment–control comparisons using non-concurrent control data (Krotka et al. (2023) &lt;doi:10.1016/j.softx.2023.101437&gt;). The package supports simulation of complex platform trial designs with continuous or binary endpoints and a flexible number of treatment arms that enter the trial at different time points. The software accommodates different treatment effects among the arms and includes several patterns for time trends. Analytic approaches currently implemented in the package cover frequentist modes (e.g., regression model adjusting for time as a fixed effect mixed model adjusting for time as a random factor, and regression splines), the Bayesian time machine a meta-analytic predictive prior separate analysis, and pooled analysis.</t>
   </si>
   <si>
-    <t>`r pkg("SIMPLE")` is a modular R package to simulate clinical trials and was developed to solve the problem of poor shareability and re-usability of existing software code in future projects (Meyer et al. (2023) &lt;10.1016/j.softx.2023.101515&gt;). In `r pkg("SIMPLE")`, different aspects of the simulation (e.g., participant recruitment, analysis strategies, and the inclusion and exclusion of further interventions into the platform) are governed by partially independent and re-usable “modules”. Due to its architecture, `r pkg("SIMPLE")` can be used as a backbone from which to create highly complex designs that are accessible to users with very limited R skills, while more advanced users can nearly infinitely tweak the designs.</t>
-  </si>
-  <si>
     <t>`r pkg("CohortPlat")` facilitates the simulation of cohort platform trials with binary endpoints, where each cohort consists of a combination treatment, the respective monotherapies, and control. Bayesian decision rules are used at the interim analysis (early futility or efficacy based on a surrogate endpoint) and at the final analysis to declare the combination therapy successful or futile. Sharing of the control and the backbone monotherapy data across cohorts is possible. The package offers extensive flexibility with respect to both platform trial trajectories, as well as treatment effect scenarios, and decision rules. This package was used to derive the simulation results in Meyer et al. (2022) &lt;doi:10.1002/pst.2194&gt;.</t>
+  </si>
+  <si>
+    <t>`r pkg("SIMPLE")` is a modular R package to simulate clinical trials and was developed to solve the problem of poor shareability and re-usability of existing software code in future projects (Meyer et al. (2023) &lt;doi:10.1016/j.softx.2023.101515&gt;). In `r pkg("SIMPLE")`, different aspects of the simulation (e.g., participant recruitment, analysis strategies, and the inclusion and exclusion of further interventions into the platform) are governed by partially independent and re-usable “modules”. Due to its architecture, `r pkg("SIMPLE")` can be used as a backbone from which to create highly complex designs that are accessible to users with very limited R skills, while more advanced users can nearly infinitely tweak the designs.</t>
   </si>
 </sst>
 </file>
@@ -1199,7 +1199,7 @@
   <dimension ref="A1:AA1004"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="C109" sqref="C109"/>
+      <selection activeCell="F118" sqref="F118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3235,7 +3235,7 @@
         <v>140</v>
       </c>
       <c r="F108" s="17" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G108" s="7"/>
     </row>
@@ -3271,7 +3271,7 @@
         <v>140</v>
       </c>
       <c r="F110" s="17" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="G110" s="7"/>
     </row>

</xml_diff>

<commit_message>
Update list of packages
</commit_message>
<xml_diff>
--- a/doc/CTV ClinicalTrial File.xlsx
+++ b/doc/CTV ClinicalTrial File.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elias/Projects/CRAN-task-view-ClinicalTrials/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D8B7340-D134-6246-AA37-52C15A9846E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0E0C42F-5B91-4E4C-B3AB-A5E0F6144F75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1020" yWindow="500" windowWidth="37380" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="271">
   <si>
     <t>Package Name</t>
   </si>
@@ -835,6 +835,12 @@
   </si>
   <si>
     <t>`r pkg("SIMPLE")` is a modular R package to simulate clinical trials and was developed to solve the problem of poor shareability and re-usability of existing software code in future projects (Meyer et al. (2023) &lt;doi:10.1016/j.softx.2023.101515&gt;). In `r pkg("SIMPLE")`, different aspects of the simulation (e.g., participant recruitment, analysis strategies, and the inclusion and exclusion of further interventions into the platform) are governed by partially independent and re-usable “modules”. Due to its architecture, `r pkg("SIMPLE")` can be used as a backbone from which to create highly complex designs that are accessible to users with very limited R skills, while more advanced users can nearly infinitely tweak the designs.</t>
+  </si>
+  <si>
+    <t>airship</t>
+  </si>
+  <si>
+    <t>`r pkg("airship")`is an R package that contains an R Shiny App designed to plot simulation results of clinical trials. Its main feature is allowing users to simultaneously investigate the impact of several simulation input dimensions through dynamic filtering of the simulation results. A more detailed description of the core app can be found in Meyer et al. (2023) &lt;doi:10.1016/j.softx.2023.101347&gt;.</t>
   </si>
 </sst>
 </file>
@@ -1199,7 +1205,7 @@
   <dimension ref="A1:AA1004"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="F118" sqref="F118"/>
+      <selection activeCell="D112" sqref="D112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3276,9 +3282,21 @@
       <c r="G110" s="7"/>
     </row>
     <row r="111" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A111" s="16"/>
-      <c r="E111" s="7"/>
-      <c r="F111" s="7"/>
+      <c r="A111" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="B111" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D111" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="E111" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="F111" s="17" t="s">
+        <v>270</v>
+      </c>
       <c r="G111" s="7"/>
     </row>
     <row r="112" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>